<commit_message>
Started to add switch cycle to print on Metel.TXT. Added an array to order data took from the excel file
</commit_message>
<xml_diff>
--- a/Metel_prova.xlsx
+++ b/Metel_prova.xlsx
@@ -16,18 +16,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>COGNOME</t>
-  </si>
-  <si>
-    <t>Mario</t>
-  </si>
-  <si>
-    <t>Ponzelli</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>Cod_Articolo</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Descri_Articolo</t>
+  </si>
+  <si>
+    <t>Pz_x_Conf</t>
+  </si>
+  <si>
+    <t>Prezzo</t>
+  </si>
+  <si>
+    <t>Famiglia</t>
+  </si>
+  <si>
+    <t>DHSHSHSDHSD</t>
+  </si>
+  <si>
+    <t>SYSEYTYETYRTY</t>
+  </si>
+  <si>
+    <t>WYRTHFGHFG</t>
+  </si>
+  <si>
+    <t>HSTHDDJHRUY</t>
+  </si>
+  <si>
+    <t>SDRGSDFGSDF</t>
+  </si>
+  <si>
+    <t>GSDFGSDFG</t>
+  </si>
+  <si>
+    <t>SDGSDFGSDFG</t>
+  </si>
+  <si>
+    <t>SDFGSDFGSDFG</t>
+  </si>
+  <si>
+    <t>SDFGSDGS</t>
   </si>
 </sst>
 </file>
@@ -63,8 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -359,35 +395,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>111111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>9.99</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>222222</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>56.2</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>333333</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>14.5</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>444444</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>555555</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>47.1</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>666666</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>56.8</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>777777</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>85</v>
+      </c>
+      <c r="F8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>888888</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>2.36</v>
+      </c>
+      <c r="F9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>999999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>1.87</v>
+      </c>
+      <c r="F10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>101010</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>55.23</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>